<commit_message>
Remove duplicate entries from form responses
</commit_message>
<xml_diff>
--- a/data/2020-06-09/SCW Weekly Comp 2020-06-09 (Responses).xlsx
+++ b/data/2020-06-09/SCW Weekly Comp 2020-06-09 (Responses).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\WCA\scw-comp\data\2020-06-09\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30EC2365-CE2C-4DC8-9FAE-EFB298C159A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2FC0817-DA55-4CFD-9A00-BEE13BAFEFCF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,14 @@
     <sheet name="Form Responses 1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Form Responses 1'!$A$1:$BW$89</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Form Responses 1'!$A$1:$BW$82</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="779" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="719" uniqueCount="302">
   <si>
     <t>Timestamp</t>
   </si>
@@ -586,9 +586,6 @@
     <t>https://www.facebook.com/events/620460455211235/permalink/622707208319893/</t>
   </si>
   <si>
-    <t>3rd attempt to be done later</t>
-  </si>
-  <si>
     <t>14:54.39</t>
   </si>
   <si>
@@ -697,12 +694,6 @@
     <t>2019THAM05</t>
   </si>
   <si>
-    <t>after second solve I accidentally did the cs timer scramble. I corrected and used the correct scramble for solve #2</t>
-  </si>
-  <si>
-    <t>Terrible avg with the new qiyi ms</t>
-  </si>
-  <si>
     <t>2:25.05</t>
   </si>
   <si>
@@ -740,9 +731,6 @@
   </si>
   <si>
     <t>https://m.facebook.com/events/903549840109576?view=permalink&amp;id=906720483125845</t>
-  </si>
-  <si>
-    <t>accidentally scrambled solve #2 with the CSTimer scramble. Corrected untimed and went on to scramble solve #2 correctly</t>
   </si>
   <si>
     <t>https://m.facebook.com/events/903549840109576?view=permalink&amp;id=906712713126622</t>
@@ -1210,14 +1198,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1">
+  <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:BW89"/>
+  <dimension ref="A1:BW82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AV1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="BE78" sqref="BE78"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1454,7 +1442,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:75" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:75" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>43991.57664248842</v>
       </c>
@@ -1495,7 +1483,7 @@
         <v>11.71</v>
       </c>
     </row>
-    <row r="3" spans="1:75" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:75" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>43991.580921562505</v>
       </c>
@@ -1536,7 +1524,7 @@
         <v>19.37</v>
       </c>
     </row>
-    <row r="4" spans="1:75" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:75" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>43991.585175405096</v>
       </c>
@@ -1577,7 +1565,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:75" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:75" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>43991.620057650463</v>
       </c>
@@ -1621,7 +1609,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:75" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:75" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>43991.640422199074</v>
       </c>
@@ -1662,7 +1650,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:75" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:75" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>43991.65705061343</v>
       </c>
@@ -1685,7 +1673,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:75" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:75" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>43991.668187754629</v>
       </c>
@@ -1729,7 +1717,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:75" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:75" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>43991.747532141206</v>
       </c>
@@ -1773,7 +1761,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="10" spans="1:75" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:75" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>43991.769298483792</v>
       </c>
@@ -1808,7 +1796,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:75" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:75" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>43991.770488622686</v>
       </c>
@@ -1843,7 +1831,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:75" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:75" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>43991.795222002314</v>
       </c>
@@ -1878,7 +1866,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:75" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:75" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>43991.823180543986</v>
       </c>
@@ -1919,7 +1907,7 @@
         <v>16.29</v>
       </c>
     </row>
-    <row r="14" spans="1:75" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:75" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>43992.439753009261</v>
       </c>
@@ -1954,7 +1942,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="15" spans="1:75" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:75" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>43992.480909340273</v>
       </c>
@@ -1995,7 +1983,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="16" spans="1:75" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:75" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>43992.49750143518</v>
       </c>
@@ -2039,7 +2027,7 @@
         <v>31.89</v>
       </c>
     </row>
-    <row r="17" spans="1:75" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:75" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>43992.562183055554</v>
       </c>
@@ -2074,7 +2062,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="18" spans="1:75" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:75" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>43992.609832060189</v>
       </c>
@@ -2109,7 +2097,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="19" spans="1:75" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:75" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>43992.61057675926</v>
       </c>
@@ -2150,7 +2138,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="20" spans="1:75" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:75" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>43992.611458506944</v>
       </c>
@@ -2191,7 +2179,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="21" spans="1:75" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:75" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>43992.697258668981</v>
       </c>
@@ -2235,7 +2223,7 @@
         <v>4.25</v>
       </c>
     </row>
-    <row r="22" spans="1:75" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:75" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>43992.69924037037</v>
       </c>
@@ -2279,7 +2267,7 @@
         <v>9.64</v>
       </c>
     </row>
-    <row r="23" spans="1:75" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:75" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>43992.701793472224</v>
       </c>
@@ -2323,7 +2311,7 @@
         <v>14.64</v>
       </c>
     </row>
-    <row r="24" spans="1:75" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:75" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>43992.743501527773</v>
       </c>
@@ -2358,7 +2346,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:75" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:75" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>43992.835891226852</v>
       </c>
@@ -2393,7 +2381,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:75" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:75" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>43992.887005532408</v>
       </c>
@@ -2416,7 +2404,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:75" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:75" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>43992.941970034721</v>
       </c>
@@ -2442,7 +2430,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:75" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:75" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>43992.972704375003</v>
       </c>
@@ -2477,7 +2465,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="1:75" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:75" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>43992.974684884262</v>
       </c>
@@ -2518,7 +2506,7 @@
         <v>50.31</v>
       </c>
     </row>
-    <row r="30" spans="1:75" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:75" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>43992.976038622684</v>
       </c>
@@ -2559,7 +2547,7 @@
         <v>7.76</v>
       </c>
     </row>
-    <row r="31" spans="1:75" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:75" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>43992.977183148148</v>
       </c>
@@ -2600,7 +2588,7 @@
         <v>18.21</v>
       </c>
     </row>
-    <row r="32" spans="1:75" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:75" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>43993.584875694447</v>
       </c>
@@ -2623,7 +2611,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:75" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:70" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>43993.69482798611</v>
       </c>
@@ -2658,7 +2646,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="34" spans="1:75" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:70" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>43993.72374616898</v>
       </c>
@@ -2693,7 +2681,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="35" spans="1:75" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:70" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>43993.73706561343</v>
       </c>
@@ -2734,7 +2722,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="36" spans="1:75" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:70" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>43993.76409261574</v>
       </c>
@@ -2775,7 +2763,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="37" spans="1:75" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:70" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>43994.121263287037</v>
       </c>
@@ -2810,7 +2798,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="38" spans="1:75" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:70" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <v>43994.176036493052</v>
       </c>
@@ -2845,7 +2833,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="39" spans="1:75" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:70" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>43994.527547881946</v>
       </c>
@@ -2886,7 +2874,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="40" spans="1:75" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:70" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>43994.765641493053</v>
       </c>
@@ -2927,9 +2915,9 @@
         <v>185</v>
       </c>
     </row>
-    <row r="41" spans="1:75" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:70" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
-        <v>43995.200325775462</v>
+        <v>43995.209666886571</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>169</v>
@@ -2941,103 +2929,106 @@
         <v>170</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="G41" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="BS41" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="BN41" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="BT41" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="BU41" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="BV41" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="BW41" s="3" t="s">
+      <c r="BO41" s="3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="42" spans="1:75" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+      <c r="BP41" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="BQ41" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="BR41" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="42" spans="1:70" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
-        <v>43995.209666886571</v>
+        <v>43995.309792141205</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>169</v>
+        <v>189</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>18</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>170</v>
+        <v>190</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>130</v>
+        <v>46</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="BN42" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="G42" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="BH42" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="BO42" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="BP42" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="BQ42" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="BR42" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="43" spans="1:75" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="43" spans="1:70" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
-        <v>43995.309792141205</v>
+        <v>43995.503767858798</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>190</v>
+        <v>48</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>18</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>191</v>
+        <v>49</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>46</v>
+        <v>23</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="G43" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="BH43" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="44" spans="1:75" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O43" s="3">
+        <v>19.260000000000002</v>
+      </c>
+      <c r="P43" s="3">
+        <v>18.61</v>
+      </c>
+      <c r="Q43" s="3">
+        <v>14.9</v>
+      </c>
+      <c r="R43" s="3">
+        <v>23.87</v>
+      </c>
+      <c r="S43" s="3">
+        <v>21.9</v>
+      </c>
+      <c r="T43" s="3">
+        <v>14.9</v>
+      </c>
+      <c r="U43" s="3">
+        <v>19.920000000000002</v>
+      </c>
+    </row>
+    <row r="44" spans="1:70" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
-        <v>43995.503767858798</v>
+        <v>43995.702823784726</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>48</v>
+        <v>132</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>18</v>
+        <v>75</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>49</v>
+        <v>133</v>
       </c>
       <c r="E44" s="3" t="s">
         <v>23</v>
@@ -3045,31 +3036,34 @@
       <c r="F44" s="4" t="s">
         <v>194</v>
       </c>
+      <c r="G44" s="3" t="s">
+        <v>195</v>
+      </c>
       <c r="O44" s="3">
-        <v>19.260000000000002</v>
+        <v>20.51</v>
       </c>
       <c r="P44" s="3">
-        <v>18.61</v>
+        <v>25.08</v>
       </c>
       <c r="Q44" s="3">
-        <v>14.9</v>
+        <v>18.510000000000002</v>
       </c>
       <c r="R44" s="3">
-        <v>23.87</v>
+        <v>15.71</v>
       </c>
       <c r="S44" s="3">
-        <v>21.9</v>
+        <v>17.95</v>
       </c>
       <c r="T44" s="3">
-        <v>14.9</v>
+        <v>15.71</v>
       </c>
       <c r="U44" s="3">
-        <v>19.920000000000002</v>
-      </c>
-    </row>
-    <row r="45" spans="1:75" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+        <v>18.989999999999998</v>
+      </c>
+    </row>
+    <row r="45" spans="1:70" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
-        <v>43995.702823784726</v>
+        <v>43995.703621516208</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>132</v>
@@ -3081,39 +3075,36 @@
         <v>133</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="G45" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="O45" s="3">
-        <v>20.51</v>
-      </c>
-      <c r="P45" s="3">
-        <v>25.08</v>
-      </c>
-      <c r="Q45" s="3">
-        <v>18.510000000000002</v>
-      </c>
-      <c r="R45" s="3">
-        <v>15.71</v>
-      </c>
-      <c r="S45" s="3">
-        <v>17.95</v>
-      </c>
-      <c r="T45" s="3">
-        <v>15.71</v>
-      </c>
-      <c r="U45" s="3">
-        <v>18.989999999999998</v>
-      </c>
-    </row>
-    <row r="46" spans="1:75" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H45" s="3">
+        <v>7.73</v>
+      </c>
+      <c r="I45" s="3">
+        <v>6.08</v>
+      </c>
+      <c r="J45" s="3">
+        <v>6.58</v>
+      </c>
+      <c r="K45" s="3">
+        <v>7.71</v>
+      </c>
+      <c r="L45" s="3">
+        <v>5.79</v>
+      </c>
+      <c r="M45" s="3">
+        <v>5.79</v>
+      </c>
+      <c r="N45" s="3">
+        <v>6.79</v>
+      </c>
+    </row>
+    <row r="46" spans="1:70" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
-        <v>43995.703621516208</v>
+        <v>43995.704918807867</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>132</v>
@@ -3125,1705 +3116,1418 @@
         <v>133</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F46" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="H46" s="3">
-        <v>7.73</v>
-      </c>
-      <c r="I46" s="3">
-        <v>6.08</v>
-      </c>
-      <c r="J46" s="3">
-        <v>6.58</v>
-      </c>
-      <c r="K46" s="3">
-        <v>7.71</v>
-      </c>
-      <c r="L46" s="3">
-        <v>5.79</v>
-      </c>
-      <c r="M46" s="3">
-        <v>5.79</v>
-      </c>
-      <c r="N46" s="3">
-        <v>6.79</v>
-      </c>
-    </row>
-    <row r="47" spans="1:75" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+      <c r="BA46" s="3">
+        <v>43.18</v>
+      </c>
+      <c r="BB46" s="3">
+        <v>44.82</v>
+      </c>
+      <c r="BC46" s="3">
+        <v>37.11</v>
+      </c>
+      <c r="BD46" s="3">
+        <v>43.93</v>
+      </c>
+      <c r="BE46" s="3">
+        <v>38.31</v>
+      </c>
+      <c r="BF46" s="3">
+        <v>37.11</v>
+      </c>
+      <c r="BG46" s="3">
+        <v>41.81</v>
+      </c>
+    </row>
+    <row r="47" spans="1:70" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
-        <v>43995.704918807867</v>
+        <v>43995.719832280098</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>132</v>
+        <v>198</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>75</v>
+        <v>18</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>133</v>
+        <v>199</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F47" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="H47" s="3">
+        <v>3.97</v>
+      </c>
+      <c r="I47" s="3">
+        <v>5.04</v>
+      </c>
+      <c r="J47" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K47" s="3">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="L47" s="3">
+        <v>4.1399999999999997</v>
+      </c>
+      <c r="M47" s="3">
+        <v>3.97</v>
+      </c>
+      <c r="N47" s="3">
+        <v>4.76</v>
+      </c>
+    </row>
+    <row r="48" spans="1:70" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A48" s="2">
+        <v>43995.722766076389</v>
+      </c>
+      <c r="B48" s="3" t="s">
         <v>198</v>
-      </c>
-      <c r="BA47" s="3">
-        <v>43.18</v>
-      </c>
-      <c r="BB47" s="3">
-        <v>44.82</v>
-      </c>
-      <c r="BC47" s="3">
-        <v>37.11</v>
-      </c>
-      <c r="BD47" s="3">
-        <v>43.93</v>
-      </c>
-      <c r="BE47" s="3">
-        <v>38.31</v>
-      </c>
-      <c r="BF47" s="3">
-        <v>37.11</v>
-      </c>
-      <c r="BG47" s="3">
-        <v>41.81</v>
-      </c>
-    </row>
-    <row r="48" spans="1:75" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="2">
-        <v>43995.719832280098</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>199</v>
       </c>
       <c r="C48" s="3" t="s">
         <v>18</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="F48" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="H48" s="3">
-        <v>3.97</v>
-      </c>
-      <c r="I48" s="3">
-        <v>5.04</v>
-      </c>
-      <c r="J48" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="K48" s="3">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="L48" s="3">
-        <v>4.1399999999999997</v>
-      </c>
-      <c r="M48" s="3">
-        <v>3.97</v>
-      </c>
-      <c r="N48" s="3">
-        <v>4.76</v>
-      </c>
-    </row>
-    <row r="49" spans="1:75" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O48" s="3">
+        <v>14.33</v>
+      </c>
+      <c r="P48" s="3">
+        <v>12</v>
+      </c>
+      <c r="Q48" s="3">
+        <v>20.94</v>
+      </c>
+      <c r="R48" s="3">
+        <v>14.82</v>
+      </c>
+      <c r="S48" s="3">
+        <v>15.04</v>
+      </c>
+      <c r="T48" s="3">
+        <v>12</v>
+      </c>
+      <c r="U48" s="3">
+        <v>14.73</v>
+      </c>
+    </row>
+    <row r="49" spans="1:75" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
-        <v>43995.722766076389</v>
+        <v>43995.72647228009</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>18</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F49" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="O49" s="3">
-        <v>14.33</v>
-      </c>
-      <c r="P49" s="3">
-        <v>12</v>
-      </c>
-      <c r="Q49" s="3">
-        <v>20.94</v>
-      </c>
-      <c r="R49" s="3">
-        <v>14.82</v>
-      </c>
-      <c r="S49" s="3">
-        <v>15.04</v>
-      </c>
-      <c r="T49" s="3">
-        <v>12</v>
-      </c>
-      <c r="U49" s="3">
-        <v>14.73</v>
-      </c>
-    </row>
-    <row r="50" spans="1:75" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+      <c r="BA49" s="3">
+        <v>23.49</v>
+      </c>
+      <c r="BB49" s="3">
+        <v>23.47</v>
+      </c>
+      <c r="BC49" s="3">
+        <v>28.48</v>
+      </c>
+      <c r="BD49" s="3">
+        <v>21.24</v>
+      </c>
+      <c r="BE49" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="BF49" s="3">
+        <v>21.24</v>
+      </c>
+      <c r="BG49" s="3">
+        <v>25.15</v>
+      </c>
+    </row>
+    <row r="50" spans="1:75" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
-        <v>43995.72647228009</v>
+        <v>43995.730772557872</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>199</v>
+        <v>132</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>18</v>
+        <v>75</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>200</v>
+        <v>133</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="F50" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="BA50" s="3">
-        <v>23.49</v>
-      </c>
-      <c r="BB50" s="3">
-        <v>23.47</v>
-      </c>
-      <c r="BC50" s="3">
-        <v>28.48</v>
-      </c>
-      <c r="BD50" s="3">
-        <v>21.24</v>
-      </c>
-      <c r="BE50" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="BF50" s="3">
-        <v>21.24</v>
-      </c>
-      <c r="BG50" s="3">
-        <v>25.15</v>
-      </c>
-    </row>
-    <row r="51" spans="1:75" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+      <c r="V50" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="W50" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="X50" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="Y50" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="Z50" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="AA50" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="AB50" s="3" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="51" spans="1:75" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
-        <v>43995.730772557872</v>
+        <v>43995.73425652778</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>132</v>
+        <v>198</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>75</v>
+        <v>18</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>133</v>
+        <v>199</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>32</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>204</v>
-      </c>
-      <c r="V51" s="3" t="s">
-        <v>205</v>
+        <v>210</v>
+      </c>
+      <c r="G51" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="V51" s="3">
+        <v>59.03</v>
       </c>
       <c r="W51" s="3" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="X51" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="Y51" s="3" t="s">
-        <v>208</v>
+        <v>213</v>
+      </c>
+      <c r="Y51" s="3">
+        <v>47.54</v>
       </c>
       <c r="Z51" s="3" t="s">
-        <v>209</v>
-      </c>
-      <c r="AA51" s="3" t="s">
-        <v>207</v>
+        <v>214</v>
+      </c>
+      <c r="AA51" s="3">
+        <v>47.54</v>
       </c>
       <c r="AB51" s="3" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="52" spans="1:75" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="52" spans="1:75" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
-        <v>43995.73425652778</v>
+        <v>43995.751124756949</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C52" s="3" t="s">
         <v>18</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>32</v>
+        <v>68</v>
       </c>
       <c r="F52" s="4" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="V52" s="3">
-        <v>59.03</v>
-      </c>
-      <c r="W52" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="X52" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="Y52" s="3">
-        <v>47.54</v>
-      </c>
-      <c r="Z52" s="3" t="s">
-        <v>215</v>
-      </c>
-      <c r="AA52" s="3">
-        <v>47.54</v>
-      </c>
-      <c r="AB52" s="3" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="53" spans="1:75" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+        <v>217</v>
+      </c>
+      <c r="AJ52" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="AK52" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="AL52" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="AM52" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="AN52" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="53" spans="1:75" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
-        <v>43995.751124756949</v>
+        <v>43995.760223773148</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>199</v>
+        <v>219</v>
       </c>
       <c r="C53" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F53" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="BH53" s="3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="54" spans="1:75" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A54" s="2">
+        <v>43995.802212812501</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="C54" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D53" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="E53" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="F53" s="4" t="s">
-        <v>217</v>
-      </c>
-      <c r="G53" s="3" t="s">
-        <v>218</v>
-      </c>
-      <c r="AJ53" s="3" t="s">
-        <v>219</v>
-      </c>
-      <c r="AK53" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="AL53" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="AM53" s="3" t="s">
-        <v>219</v>
-      </c>
-      <c r="AN53" s="3" t="s">
+      <c r="D54" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="F54" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="BS54" s="3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="54" spans="1:75" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="2">
-        <v>43995.760223773148</v>
-      </c>
-      <c r="B54" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="C54" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="E54" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="F54" s="4" t="s">
-        <v>221</v>
-      </c>
-      <c r="BH54" s="3">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="55" spans="1:75" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+      <c r="BT54" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="BU54" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="BV54" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="BW54" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="55" spans="1:75" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
-        <v>43995.794020277783</v>
+        <v>43995.804535000003</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>222</v>
+        <v>74</v>
       </c>
       <c r="C55" s="3" t="s">
         <v>75</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>223</v>
+        <v>76</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G55" s="3" t="s">
-        <v>224</v>
-      </c>
-      <c r="O55" s="3">
-        <v>30.25</v>
-      </c>
-      <c r="P55" s="3">
-        <v>30.58</v>
-      </c>
-      <c r="Q55" s="3">
-        <v>46.47</v>
-      </c>
-      <c r="R55" s="3">
-        <v>26.69</v>
-      </c>
-      <c r="S55" s="3">
-        <v>32.770000000000003</v>
-      </c>
-      <c r="T55" s="3">
-        <v>26.69</v>
-      </c>
-      <c r="U55" s="3">
-        <v>31.2</v>
-      </c>
-    </row>
-    <row r="56" spans="1:75" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+      <c r="F55" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="H55" s="3">
+        <v>12.63</v>
+      </c>
+      <c r="I55" s="3">
+        <v>16.71</v>
+      </c>
+      <c r="J55" s="3">
+        <v>13.9</v>
+      </c>
+      <c r="K55" s="3">
+        <v>13.77</v>
+      </c>
+      <c r="L55" s="3">
+        <v>18.13</v>
+      </c>
+      <c r="M55" s="3">
+        <v>12.63</v>
+      </c>
+      <c r="N55" s="3">
+        <v>14.79</v>
+      </c>
+    </row>
+    <row r="56" spans="1:75" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
-        <v>43995.795861574079</v>
+        <v>43995.806013055553</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>222</v>
+        <v>74</v>
       </c>
       <c r="C56" s="3" t="s">
         <v>75</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>223</v>
+        <v>76</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G56" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="H56" s="3">
-        <v>10.48</v>
-      </c>
-      <c r="I56" s="3">
-        <v>13.11</v>
-      </c>
-      <c r="J56" s="3">
-        <v>8.52</v>
-      </c>
-      <c r="K56" s="3">
-        <v>12.15</v>
-      </c>
-      <c r="L56" s="3">
-        <v>17.04</v>
-      </c>
-      <c r="M56" s="3">
-        <v>8.52</v>
-      </c>
-      <c r="N56" s="3">
-        <v>11.91</v>
-      </c>
-    </row>
-    <row r="57" spans="1:75" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+      <c r="F56" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="BA56" s="3">
+        <v>56.61</v>
+      </c>
+      <c r="BB56" s="3">
+        <v>59.91</v>
+      </c>
+      <c r="BC56" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="BD56" s="3">
+        <v>57.36</v>
+      </c>
+      <c r="BE56" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="BF56" s="3">
+        <v>56.61</v>
+      </c>
+      <c r="BG56" s="3" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="57" spans="1:75" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
-        <v>43995.796859016205</v>
+        <v>43995.807349803239</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>222</v>
+        <v>74</v>
       </c>
       <c r="C57" s="3" t="s">
         <v>75</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>223</v>
+        <v>76</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="V57" s="3" t="s">
-        <v>226</v>
-      </c>
-      <c r="W57" s="3" t="s">
-        <v>227</v>
-      </c>
-      <c r="X57" s="3" t="s">
-        <v>228</v>
-      </c>
-      <c r="Y57" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="Z57" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="AA57" s="3" t="s">
-        <v>227</v>
-      </c>
-      <c r="AB57" s="3" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="58" spans="1:75" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+      <c r="F57" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="O57" s="3">
+        <v>23</v>
+      </c>
+      <c r="P57" s="3">
+        <v>20.49</v>
+      </c>
+      <c r="Q57" s="3">
+        <v>18.14</v>
+      </c>
+      <c r="R57" s="3">
+        <v>17.61</v>
+      </c>
+      <c r="S57" s="3">
+        <v>23.31</v>
+      </c>
+      <c r="T57" s="3">
+        <v>17.61</v>
+      </c>
+      <c r="U57" s="3">
+        <v>20.54</v>
+      </c>
+    </row>
+    <row r="58" spans="1:75" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
-        <v>43995.797632858797</v>
+        <v>43995.838484594904</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C58" s="3" t="s">
         <v>75</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="AC58" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="AD58" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="AE58" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="AF58" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="AG58" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="AH58" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="AI58" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="59" spans="1:75" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+      <c r="F58" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="G58" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="O58" s="3">
+        <v>30.25</v>
+      </c>
+      <c r="P58" s="3">
+        <v>30.58</v>
+      </c>
+      <c r="Q58" s="3">
+        <v>46.47</v>
+      </c>
+      <c r="R58" s="3">
+        <v>26.69</v>
+      </c>
+      <c r="S58" s="3">
+        <v>32.770000000000003</v>
+      </c>
+      <c r="T58" s="3">
+        <v>26.69</v>
+      </c>
+      <c r="U58" s="3">
+        <v>31.2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:75" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A59" s="2">
-        <v>43995.798344733797</v>
+        <v>43995.839606400463</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C59" s="3" t="s">
         <v>75</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E59" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F59" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="G59" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="H59" s="3">
+        <v>10.48</v>
+      </c>
+      <c r="I59" s="3">
+        <v>13.11</v>
+      </c>
+      <c r="J59" s="3">
+        <v>8.52</v>
+      </c>
+      <c r="K59" s="3">
+        <v>12.15</v>
+      </c>
+      <c r="L59" s="3">
+        <v>17.04</v>
+      </c>
+      <c r="M59" s="3">
+        <v>8.52</v>
+      </c>
+      <c r="N59" s="3">
+        <v>11.91</v>
+      </c>
+    </row>
+    <row r="60" spans="1:75" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A60" s="2">
+        <v>43995.840662499999</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="E60" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="AT59" s="3" t="s">
-        <v>231</v>
-      </c>
-      <c r="AU59" s="3" t="s">
+      <c r="F60" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="G60" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="AT60" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="AU60" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="AV59" s="3" t="s">
+      <c r="AV60" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="AW59" s="3" t="s">
+      <c r="AW60" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="AX59" s="3" t="s">
+      <c r="AX60" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="AY59" s="3" t="s">
-        <v>231</v>
-      </c>
-      <c r="AZ59" s="3" t="s">
+      <c r="AY60" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="AZ60" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="60" spans="1:75" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="2">
-        <v>43995.802212812501</v>
-      </c>
-      <c r="B60" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="C60" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D60" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="E60" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="F60" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="BS60" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="BT60" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="BU60" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="BV60" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="BW60" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="61" spans="1:75" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:75" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A61" s="2">
-        <v>43995.804535000003</v>
+        <v>43995.841845590279</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>74</v>
+        <v>221</v>
       </c>
       <c r="C61" s="3" t="s">
         <v>75</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>76</v>
+        <v>222</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="F61" s="4" t="s">
-        <v>232</v>
-      </c>
-      <c r="H61" s="3">
-        <v>12.63</v>
-      </c>
-      <c r="I61" s="3">
-        <v>16.71</v>
-      </c>
-      <c r="J61" s="3">
-        <v>13.9</v>
-      </c>
-      <c r="K61" s="3">
-        <v>13.77</v>
-      </c>
-      <c r="L61" s="3">
-        <v>18.13</v>
-      </c>
-      <c r="M61" s="3">
-        <v>12.63</v>
-      </c>
-      <c r="N61" s="3">
-        <v>14.79</v>
-      </c>
-    </row>
-    <row r="62" spans="1:75" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+        <v>241</v>
+      </c>
+      <c r="V61" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="W61" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="X61" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="Y61" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z61" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA61" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="AB61" s="3" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="62" spans="1:75" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A62" s="2">
-        <v>43995.806013055553</v>
+        <v>43995.842700104171</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>74</v>
+        <v>221</v>
       </c>
       <c r="C62" s="3" t="s">
         <v>75</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>76</v>
+        <v>222</v>
       </c>
       <c r="E62" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="F62" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="AC62" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="AD62" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="AE62" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF62" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="AG62" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="AH62" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="AI62" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="63" spans="1:75" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A63" s="2">
+        <v>43996.008762592595</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="E63" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F63" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="G63" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="BH63" s="3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="64" spans="1:75" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A64" s="2">
+        <v>43996.088817604163</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="E64" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F64" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="H64" s="3">
+        <v>9.4700000000000006</v>
+      </c>
+      <c r="I64" s="3">
+        <v>8.9700000000000006</v>
+      </c>
+      <c r="J64" s="3">
+        <v>10.5</v>
+      </c>
+      <c r="K64" s="3">
+        <v>10.29</v>
+      </c>
+      <c r="L64" s="3">
+        <v>11.48</v>
+      </c>
+      <c r="M64" s="3">
+        <v>8.9700000000000006</v>
+      </c>
+      <c r="N64" s="3">
+        <v>10.09</v>
+      </c>
+    </row>
+    <row r="65" spans="1:65" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A65" s="2">
+        <v>43996.593975914351</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E65" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="F62" s="4" t="s">
-        <v>233</v>
-      </c>
-      <c r="BA62" s="3">
-        <v>56.61</v>
-      </c>
-      <c r="BB62" s="3">
-        <v>59.91</v>
-      </c>
-      <c r="BC62" s="3" t="s">
-        <v>234</v>
-      </c>
-      <c r="BD62" s="3">
-        <v>57.36</v>
-      </c>
-      <c r="BE62" s="3" t="s">
-        <v>235</v>
-      </c>
-      <c r="BF62" s="3">
-        <v>56.61</v>
-      </c>
-      <c r="BG62" s="3" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="63" spans="1:75" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="2">
-        <v>43995.807349803239</v>
-      </c>
-      <c r="B63" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C63" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="D63" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="E63" s="3" t="s">
+      <c r="F65" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="BA65" s="3">
+        <v>35.25</v>
+      </c>
+      <c r="BB65" s="3">
+        <v>33.15</v>
+      </c>
+      <c r="BC65" s="3">
+        <v>26.13</v>
+      </c>
+      <c r="BD65" s="3">
+        <v>54.33</v>
+      </c>
+      <c r="BE65" s="3">
+        <v>26.61</v>
+      </c>
+      <c r="BF65" s="3">
+        <v>26.13</v>
+      </c>
+      <c r="BG65" s="3">
+        <v>31.67</v>
+      </c>
+    </row>
+    <row r="66" spans="1:65" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A66" s="2">
+        <v>43996.694791377318</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="E66" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F63" s="4" t="s">
-        <v>237</v>
-      </c>
-      <c r="O63" s="3">
-        <v>23</v>
-      </c>
-      <c r="P63" s="3">
-        <v>20.49</v>
-      </c>
-      <c r="Q63" s="3">
-        <v>18.14</v>
-      </c>
-      <c r="R63" s="3">
-        <v>17.61</v>
-      </c>
-      <c r="S63" s="3">
-        <v>23.31</v>
-      </c>
-      <c r="T63" s="3">
-        <v>17.61</v>
-      </c>
-      <c r="U63" s="3">
-        <v>20.54</v>
-      </c>
-    </row>
-    <row r="64" spans="1:75" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="2">
-        <v>43995.836963159723</v>
-      </c>
-      <c r="B64" s="3" t="s">
-        <v>222</v>
-      </c>
-      <c r="C64" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="D64" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="E64" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F64" s="4" t="s">
-        <v>238</v>
-      </c>
-      <c r="G64" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="O64" s="3">
-        <v>30.25</v>
-      </c>
-      <c r="P64" s="3">
-        <v>30.58</v>
-      </c>
-      <c r="Q64" s="3">
-        <v>46.47</v>
-      </c>
-      <c r="R64" s="3">
-        <v>26.69</v>
-      </c>
-      <c r="S64" s="3">
-        <v>32.770000000000003</v>
-      </c>
-      <c r="T64" s="3">
-        <v>26.69</v>
-      </c>
-      <c r="U64" s="3">
-        <v>31.2</v>
-      </c>
-    </row>
-    <row r="65" spans="1:60" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="2">
-        <v>43995.838484594904</v>
-      </c>
-      <c r="B65" s="3" t="s">
-        <v>222</v>
-      </c>
-      <c r="C65" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="D65" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="E65" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F65" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="G65" s="3" t="s">
-        <v>241</v>
-      </c>
-      <c r="O65" s="3">
-        <v>30.25</v>
-      </c>
-      <c r="P65" s="3">
-        <v>30.58</v>
-      </c>
-      <c r="Q65" s="3">
-        <v>46.47</v>
-      </c>
-      <c r="R65" s="3">
-        <v>26.69</v>
-      </c>
-      <c r="S65" s="3">
-        <v>32.770000000000003</v>
-      </c>
-      <c r="T65" s="3">
-        <v>26.69</v>
-      </c>
-      <c r="U65" s="3">
-        <v>31.2</v>
-      </c>
-    </row>
-    <row r="66" spans="1:60" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="2">
-        <v>43995.839606400463</v>
-      </c>
-      <c r="B66" s="3" t="s">
-        <v>222</v>
-      </c>
-      <c r="C66" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="D66" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="E66" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="F66" s="4" t="s">
-        <v>242</v>
-      </c>
-      <c r="G66" s="3" t="s">
-        <v>243</v>
-      </c>
-      <c r="H66" s="3">
-        <v>10.48</v>
-      </c>
-      <c r="I66" s="3">
-        <v>13.11</v>
-      </c>
-      <c r="J66" s="3">
-        <v>8.52</v>
-      </c>
-      <c r="K66" s="3">
-        <v>12.15</v>
-      </c>
-      <c r="L66" s="3">
-        <v>17.04</v>
-      </c>
-      <c r="M66" s="3">
-        <v>8.52</v>
-      </c>
-      <c r="N66" s="3">
-        <v>11.91</v>
-      </c>
-    </row>
-    <row r="67" spans="1:60" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+        <v>251</v>
+      </c>
+      <c r="O66" s="3">
+        <v>16.93</v>
+      </c>
+      <c r="P66" s="3">
+        <v>17.809999999999999</v>
+      </c>
+      <c r="Q66" s="3">
+        <v>19.899999999999999</v>
+      </c>
+      <c r="R66" s="3">
+        <v>22.3</v>
+      </c>
+      <c r="S66" s="3">
+        <v>15.69</v>
+      </c>
+      <c r="T66" s="3">
+        <v>15.69</v>
+      </c>
+      <c r="U66" s="3">
+        <v>18.21</v>
+      </c>
+    </row>
+    <row r="67" spans="1:65" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A67" s="2">
-        <v>43995.840662499999</v>
+        <v>43996.791756458333</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C67" s="3" t="s">
         <v>75</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E67" s="3" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="F67" s="4" t="s">
-        <v>238</v>
+        <v>252</v>
       </c>
       <c r="G67" s="3" t="s">
-        <v>244</v>
-      </c>
-      <c r="AT67" s="3" t="s">
-        <v>231</v>
-      </c>
-      <c r="AU67" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="BA67" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="BB67" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="BC67" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="BD67" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="AV67" s="3" t="s">
+      <c r="BE67" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="AW67" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="AX67" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="AY67" s="3" t="s">
-        <v>231</v>
-      </c>
-      <c r="AZ67" s="3" t="s">
+      <c r="BF67" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="BG67" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="68" spans="1:65" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A68" s="2">
+        <v>43997.516130798613</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="E68" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F68" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="O68" s="3">
+        <v>23.92</v>
+      </c>
+      <c r="P68" s="3">
+        <v>26.86</v>
+      </c>
+      <c r="Q68" s="3">
+        <v>25.23</v>
+      </c>
+      <c r="R68" s="3">
+        <v>33.39</v>
+      </c>
+      <c r="S68" s="3">
+        <v>27.05</v>
+      </c>
+      <c r="T68" s="3">
+        <v>23.92</v>
+      </c>
+      <c r="U68" s="3">
+        <v>26.38</v>
+      </c>
+    </row>
+    <row r="69" spans="1:65" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A69" s="2">
+        <v>43997.544250127314</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="D69" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="E69" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F69" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="BH69" s="3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="70" spans="1:65" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A70" s="2">
+        <v>43997.56983896991</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="E70" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F70" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="O70" s="3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="68" spans="1:60" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="2">
-        <v>43995.841845590279</v>
-      </c>
-      <c r="B68" s="3" t="s">
-        <v>222</v>
-      </c>
-      <c r="C68" s="3" t="s">
+      <c r="P70" s="3">
+        <v>22.65</v>
+      </c>
+      <c r="Q70" s="3">
+        <v>17.16</v>
+      </c>
+      <c r="R70" s="3">
+        <v>28.87</v>
+      </c>
+      <c r="S70" s="3">
+        <v>16.11</v>
+      </c>
+      <c r="T70" s="3">
+        <v>16.11</v>
+      </c>
+      <c r="U70" s="3">
+        <v>22.89</v>
+      </c>
+    </row>
+    <row r="71" spans="1:65" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A71" s="2">
+        <v>43997.571044733791</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="C71" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="D68" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="E68" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F68" s="4" t="s">
-        <v>245</v>
-      </c>
-      <c r="V68" s="3" t="s">
-        <v>226</v>
-      </c>
-      <c r="W68" s="3" t="s">
-        <v>227</v>
-      </c>
-      <c r="X68" s="3" t="s">
-        <v>228</v>
-      </c>
-      <c r="Y68" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="Z68" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="AA68" s="3" t="s">
-        <v>227</v>
-      </c>
-      <c r="AB68" s="3" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="69" spans="1:60" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="2">
-        <v>43995.842700104171</v>
-      </c>
-      <c r="B69" s="3" t="s">
-        <v>222</v>
-      </c>
-      <c r="C69" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="D69" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="E69" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="F69" s="4" t="s">
-        <v>246</v>
-      </c>
-      <c r="AC69" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="AD69" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="AE69" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="AF69" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="AG69" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="AH69" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="AI69" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="70" spans="1:60" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="2">
-        <v>43996.008762592595</v>
-      </c>
-      <c r="B70" s="3" t="s">
-        <v>247</v>
-      </c>
-      <c r="C70" s="3" t="s">
-        <v>248</v>
-      </c>
-      <c r="E70" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="F70" s="4" t="s">
-        <v>249</v>
-      </c>
-      <c r="G70" s="3" t="s">
-        <v>250</v>
-      </c>
-      <c r="BH70" s="3">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="71" spans="1:60" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="2">
-        <v>43996.088817604163</v>
-      </c>
-      <c r="B71" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="C71" s="3" t="s">
-        <v>18</v>
-      </c>
       <c r="D71" s="3" t="s">
-        <v>92</v>
+        <v>265</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F71" s="4" t="s">
-        <v>251</v>
-      </c>
-      <c r="H71" s="3">
-        <v>9.4700000000000006</v>
-      </c>
-      <c r="I71" s="3">
-        <v>8.9700000000000006</v>
-      </c>
-      <c r="J71" s="3">
-        <v>10.5</v>
-      </c>
-      <c r="K71" s="3">
-        <v>10.29</v>
-      </c>
-      <c r="L71" s="3">
-        <v>11.48</v>
-      </c>
-      <c r="M71" s="3">
-        <v>8.9700000000000006</v>
-      </c>
-      <c r="N71" s="3">
-        <v>10.09</v>
-      </c>
-    </row>
-    <row r="72" spans="1:60" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+        <v>267</v>
+      </c>
+      <c r="BA71" s="3">
+        <v>22.89</v>
+      </c>
+      <c r="BB71" s="3">
+        <v>24.15</v>
+      </c>
+      <c r="BC71" s="3">
+        <v>26.65</v>
+      </c>
+      <c r="BD71" s="3">
+        <v>24.15</v>
+      </c>
+      <c r="BE71" s="3">
+        <v>23.18</v>
+      </c>
+      <c r="BF71" s="3">
+        <v>22.89</v>
+      </c>
+      <c r="BG71" s="3">
+        <v>23.83</v>
+      </c>
+    </row>
+    <row r="72" spans="1:65" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A72" s="2">
-        <v>43996.593975914351</v>
+        <v>43997.717956192129</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>48</v>
+        <v>198</v>
       </c>
       <c r="C72" s="3" t="s">
         <v>18</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>49</v>
+        <v>199</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>25</v>
+        <v>46</v>
       </c>
       <c r="F72" s="4" t="s">
-        <v>252</v>
-      </c>
-      <c r="BA72" s="3">
-        <v>35.25</v>
-      </c>
-      <c r="BB72" s="3">
-        <v>33.15</v>
-      </c>
-      <c r="BC72" s="3">
-        <v>26.13</v>
-      </c>
-      <c r="BD72" s="3">
-        <v>54.33</v>
-      </c>
-      <c r="BE72" s="3">
-        <v>26.61</v>
-      </c>
-      <c r="BF72" s="3">
-        <v>26.13</v>
-      </c>
-      <c r="BG72" s="3">
-        <v>31.67</v>
-      </c>
-    </row>
-    <row r="73" spans="1:60" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+        <v>268</v>
+      </c>
+      <c r="BH72" s="3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="73" spans="1:65" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A73" s="2">
-        <v>43996.694791377318</v>
+        <v>43997.728737789352</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>253</v>
+        <v>198</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>254</v>
+        <v>18</v>
+      </c>
+      <c r="D73" s="3" t="s">
+        <v>199</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>23</v>
+        <v>105</v>
       </c>
       <c r="F73" s="4" t="s">
-        <v>255</v>
-      </c>
-      <c r="O73" s="3">
-        <v>16.93</v>
-      </c>
-      <c r="P73" s="3">
-        <v>17.809999999999999</v>
-      </c>
-      <c r="Q73" s="3">
-        <v>19.899999999999999</v>
-      </c>
-      <c r="R73" s="3">
-        <v>22.3</v>
-      </c>
-      <c r="S73" s="3">
-        <v>15.69</v>
-      </c>
-      <c r="T73" s="3">
-        <v>15.69</v>
-      </c>
-      <c r="U73" s="3">
-        <v>18.21</v>
-      </c>
-    </row>
-    <row r="74" spans="1:60" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+        <v>269</v>
+      </c>
+      <c r="G73" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="AC73" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="AD73" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="AE73" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="AF73" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="AG73" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="AH73" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="AI73" s="3" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="74" spans="1:65" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A74" s="2">
-        <v>43996.791756458333</v>
+        <v>43997.890856111109</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>222</v>
+        <v>277</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>75</v>
+        <v>18</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>223</v>
+        <v>278</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>25</v>
+        <v>153</v>
       </c>
       <c r="F74" s="4" t="s">
-        <v>256</v>
-      </c>
-      <c r="G74" s="3" t="s">
-        <v>257</v>
-      </c>
-      <c r="BA74" s="3" t="s">
-        <v>258</v>
-      </c>
-      <c r="BB74" s="3" t="s">
-        <v>259</v>
-      </c>
-      <c r="BC74" s="3" t="s">
-        <v>260</v>
-      </c>
-      <c r="BD74" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="BE74" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="BF74" s="3" t="s">
-        <v>258</v>
-      </c>
-      <c r="BG74" s="3" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="75" spans="1:60" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+        <v>279</v>
+      </c>
+      <c r="BI74" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="BJ74" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="BK74" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="BL74" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="BM74" s="3" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="75" spans="1:65" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A75" s="2">
-        <v>43997.516130798613</v>
+        <v>43997.892144791665</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>263</v>
+        <v>18</v>
+      </c>
+      <c r="D75" s="3" t="s">
+        <v>278</v>
       </c>
       <c r="E75" s="3" t="s">
         <v>23</v>
       </c>
       <c r="F75" s="4" t="s">
-        <v>264</v>
+        <v>284</v>
       </c>
       <c r="O75" s="3">
-        <v>23.92</v>
+        <v>17.68</v>
       </c>
       <c r="P75" s="3">
-        <v>26.86</v>
+        <v>18.77</v>
       </c>
       <c r="Q75" s="3">
-        <v>25.23</v>
+        <v>19.2</v>
       </c>
       <c r="R75" s="3">
-        <v>33.39</v>
+        <v>22.7</v>
       </c>
       <c r="S75" s="3">
-        <v>27.05</v>
+        <v>29.83</v>
       </c>
       <c r="T75" s="3">
-        <v>23.92</v>
+        <v>17.68</v>
       </c>
       <c r="U75" s="3">
-        <v>26.38</v>
-      </c>
-    </row>
-    <row r="76" spans="1:60" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+        <v>20.22</v>
+      </c>
+    </row>
+    <row r="76" spans="1:65" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A76" s="2">
-        <v>43997.544250127314</v>
+        <v>43997.893238958335</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>265</v>
+        <v>277</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>263</v>
+        <v>18</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>266</v>
+        <v>278</v>
       </c>
       <c r="E76" s="3" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="F76" s="4" t="s">
-        <v>267</v>
-      </c>
-      <c r="BH76" s="3">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="77" spans="1:60" ht="12.75" x14ac:dyDescent="0.2">
+        <v>285</v>
+      </c>
+      <c r="BA76" s="3">
+        <v>38.630000000000003</v>
+      </c>
+      <c r="BB76" s="3">
+        <v>34.24</v>
+      </c>
+      <c r="BC76" s="3">
+        <v>43.14</v>
+      </c>
+      <c r="BD76" s="3">
+        <v>40.590000000000003</v>
+      </c>
+      <c r="BE76" s="3">
+        <v>33.07</v>
+      </c>
+      <c r="BF76" s="3">
+        <v>33.07</v>
+      </c>
+      <c r="BG76" s="3">
+        <v>37.82</v>
+      </c>
+    </row>
+    <row r="77" spans="1:65" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A77" s="2">
-        <v>43997.56983896991</v>
+        <v>43997.928054432872</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>268</v>
+        <v>286</v>
       </c>
       <c r="C77" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="D77" s="3" t="s">
-        <v>269</v>
-      </c>
       <c r="E77" s="3" t="s">
         <v>23</v>
       </c>
       <c r="F77" s="4" t="s">
-        <v>270</v>
-      </c>
-      <c r="O77" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="O77" s="3">
+        <v>25.96</v>
+      </c>
+      <c r="P77" s="3">
+        <v>20.420000000000002</v>
+      </c>
+      <c r="Q77" s="3">
+        <v>22.52</v>
+      </c>
+      <c r="R77" s="3">
+        <v>32.1</v>
+      </c>
+      <c r="S77" s="3">
+        <v>20.84</v>
+      </c>
+      <c r="T77" s="3">
+        <v>20.420000000000002</v>
+      </c>
+      <c r="U77" s="3">
+        <v>23.1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:65" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A78" s="2">
+        <v>43997.979611574076</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="D78" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="E78" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F78" s="4" t="s">
+        <v>290</v>
+      </c>
+      <c r="H78" s="3">
+        <v>7.67</v>
+      </c>
+      <c r="I78" s="3">
+        <v>8.3800000000000008</v>
+      </c>
+      <c r="J78" s="3">
+        <v>19.71</v>
+      </c>
+      <c r="K78" s="3">
+        <v>8.52</v>
+      </c>
+      <c r="L78" s="3">
+        <v>6.54</v>
+      </c>
+      <c r="M78" s="3">
+        <v>6.54</v>
+      </c>
+      <c r="N78" s="3">
+        <v>8.19</v>
+      </c>
+    </row>
+    <row r="79" spans="1:65" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A79" s="2">
+        <v>43997.980538414355</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="C79" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="D79" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="E79" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F79" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="O79" s="3">
+        <v>27.02</v>
+      </c>
+      <c r="P79" s="3">
+        <v>27.53</v>
+      </c>
+      <c r="Q79" s="3">
+        <v>29.19</v>
+      </c>
+      <c r="R79" s="3">
+        <v>25.4</v>
+      </c>
+      <c r="S79" s="3">
+        <v>27.52</v>
+      </c>
+      <c r="T79" s="3">
+        <v>25.4</v>
+      </c>
+      <c r="U79" s="3">
+        <v>27.36</v>
+      </c>
+    </row>
+    <row r="80" spans="1:65" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A80" s="2">
+        <v>43998.339227928242</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="C80" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="E80" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="F80" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="G80" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="BI80" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="P77" s="3">
-        <v>22.65</v>
-      </c>
-      <c r="Q77" s="3">
-        <v>17.16</v>
-      </c>
-      <c r="R77" s="3">
-        <v>28.87</v>
-      </c>
-      <c r="S77" s="3">
-        <v>16.11</v>
-      </c>
-      <c r="T77" s="3">
-        <v>16.11</v>
-      </c>
-      <c r="U77" s="3">
-        <v>22.89</v>
-      </c>
-    </row>
-    <row r="78" spans="1:60" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A78" s="2">
-        <v>43997.571044733791</v>
-      </c>
-      <c r="B78" s="3" t="s">
-        <v>268</v>
-      </c>
-      <c r="C78" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="D78" s="3" t="s">
-        <v>269</v>
-      </c>
-      <c r="E78" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F78" s="4" t="s">
-        <v>271</v>
-      </c>
-      <c r="BA78" s="3">
-        <v>22.89</v>
-      </c>
-      <c r="BB78" s="3">
-        <v>24.15</v>
-      </c>
-      <c r="BC78" s="3">
-        <v>26.65</v>
-      </c>
-      <c r="BD78" s="3">
-        <v>24.15</v>
-      </c>
-      <c r="BE78" s="3">
-        <v>23.18</v>
-      </c>
-      <c r="BF78" s="3">
-        <v>22.89</v>
-      </c>
-      <c r="BG78" s="3">
-        <v>23.83</v>
-      </c>
-    </row>
-    <row r="79" spans="1:60" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="2">
-        <v>43997.717956192129</v>
-      </c>
-      <c r="B79" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="C79" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D79" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="E79" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="F79" s="4" t="s">
-        <v>272</v>
-      </c>
-      <c r="BH79" s="3">
+      <c r="BJ80" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="BK80" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="BL80" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="BM80" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="81" spans="1:28" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A81" s="2">
+        <v>43998.340830671295</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="E81" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F81" s="4" t="s">
+        <v>296</v>
+      </c>
+      <c r="O81" s="3">
+        <v>51.54</v>
+      </c>
+      <c r="P81" s="3">
+        <v>35.299999999999997</v>
+      </c>
+      <c r="Q81" s="3">
+        <v>35.11</v>
+      </c>
+      <c r="R81" s="3">
+        <v>32.979999999999997</v>
+      </c>
+      <c r="S81" s="3">
+        <v>28.59</v>
+      </c>
+      <c r="T81" s="3">
+        <v>28.59</v>
+      </c>
+      <c r="U81" s="3">
+        <v>34.46</v>
+      </c>
+    </row>
+    <row r="82" spans="1:28" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A82" s="2">
+        <v>43998.341803854171</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="E82" s="3" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="80" spans="1:60" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="2">
-        <v>43997.728737789352</v>
-      </c>
-      <c r="B80" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="C80" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D80" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="E80" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="F80" s="4" t="s">
-        <v>273</v>
-      </c>
-      <c r="G80" s="3" t="s">
-        <v>274</v>
-      </c>
-      <c r="AC80" s="3" t="s">
-        <v>275</v>
-      </c>
-      <c r="AD80" s="3" t="s">
-        <v>276</v>
-      </c>
-      <c r="AE80" s="3" t="s">
-        <v>277</v>
-      </c>
-      <c r="AF80" s="3" t="s">
-        <v>278</v>
-      </c>
-      <c r="AG80" s="3" t="s">
-        <v>279</v>
-      </c>
-      <c r="AH80" s="3" t="s">
-        <v>279</v>
-      </c>
-      <c r="AI80" s="3" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="81" spans="1:65" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="2">
-        <v>43997.890856111109</v>
-      </c>
-      <c r="B81" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="C81" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D81" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="E81" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="F81" s="4" t="s">
-        <v>283</v>
-      </c>
-      <c r="BI81" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="BJ81" s="3" t="s">
-        <v>285</v>
-      </c>
-      <c r="BK81" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="BL81" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="BM81" s="3" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="82" spans="1:65" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="2">
-        <v>43997.892144791665</v>
-      </c>
-      <c r="B82" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="C82" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D82" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="E82" s="3" t="s">
-        <v>23</v>
-      </c>
       <c r="F82" s="4" t="s">
-        <v>288</v>
-      </c>
-      <c r="O82" s="3">
-        <v>17.68</v>
-      </c>
-      <c r="P82" s="3">
-        <v>18.77</v>
-      </c>
-      <c r="Q82" s="3">
-        <v>19.2</v>
-      </c>
-      <c r="R82" s="3">
-        <v>22.7</v>
-      </c>
-      <c r="S82" s="3">
-        <v>29.83</v>
-      </c>
-      <c r="T82" s="3">
-        <v>17.68</v>
-      </c>
-      <c r="U82" s="3">
-        <v>20.22</v>
-      </c>
-    </row>
-    <row r="83" spans="1:65" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="2">
-        <v>43997.893238958335</v>
-      </c>
-      <c r="B83" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="C83" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D83" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="E83" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F83" s="4" t="s">
-        <v>289</v>
-      </c>
-      <c r="BA83" s="3">
-        <v>38.630000000000003</v>
-      </c>
-      <c r="BB83" s="3">
-        <v>34.24</v>
-      </c>
-      <c r="BC83" s="3">
-        <v>43.14</v>
-      </c>
-      <c r="BD83" s="3">
-        <v>40.590000000000003</v>
-      </c>
-      <c r="BE83" s="3">
-        <v>33.07</v>
-      </c>
-      <c r="BF83" s="3">
-        <v>33.07</v>
-      </c>
-      <c r="BG83" s="3">
-        <v>37.82</v>
-      </c>
-    </row>
-    <row r="84" spans="1:65" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="2">
-        <v>43997.928054432872</v>
-      </c>
-      <c r="B84" s="3" t="s">
-        <v>290</v>
-      </c>
-      <c r="C84" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="E84" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F84" s="4" t="s">
-        <v>291</v>
-      </c>
-      <c r="O84" s="3">
-        <v>25.96</v>
-      </c>
-      <c r="P84" s="3">
-        <v>20.420000000000002</v>
-      </c>
-      <c r="Q84" s="3">
-        <v>22.52</v>
-      </c>
-      <c r="R84" s="3">
-        <v>32.1</v>
-      </c>
-      <c r="S84" s="3">
-        <v>20.84</v>
-      </c>
-      <c r="T84" s="3">
-        <v>20.420000000000002</v>
-      </c>
-      <c r="U84" s="3">
-        <v>23.1</v>
-      </c>
-    </row>
-    <row r="85" spans="1:65" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="2">
-        <v>43997.979611574076</v>
-      </c>
-      <c r="B85" s="3" t="s">
-        <v>292</v>
-      </c>
-      <c r="C85" s="3" t="s">
-        <v>263</v>
-      </c>
-      <c r="D85" s="3" t="s">
-        <v>293</v>
-      </c>
-      <c r="E85" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F85" s="4" t="s">
-        <v>294</v>
-      </c>
-      <c r="H85" s="3">
-        <v>7.67</v>
-      </c>
-      <c r="I85" s="3">
-        <v>8.3800000000000008</v>
-      </c>
-      <c r="J85" s="3">
-        <v>19.71</v>
-      </c>
-      <c r="K85" s="3">
-        <v>8.52</v>
-      </c>
-      <c r="L85" s="3">
-        <v>6.54</v>
-      </c>
-      <c r="M85" s="3">
-        <v>6.54</v>
-      </c>
-      <c r="N85" s="3">
-        <v>8.19</v>
-      </c>
-    </row>
-    <row r="86" spans="1:65" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="2">
-        <v>43997.980538414355</v>
-      </c>
-      <c r="B86" s="3" t="s">
-        <v>292</v>
-      </c>
-      <c r="C86" s="3" t="s">
-        <v>263</v>
-      </c>
-      <c r="D86" s="3" t="s">
-        <v>293</v>
-      </c>
-      <c r="E86" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F86" s="4" t="s">
-        <v>295</v>
-      </c>
-      <c r="O86" s="3">
-        <v>27.02</v>
-      </c>
-      <c r="P86" s="3">
-        <v>27.53</v>
-      </c>
-      <c r="Q86" s="3">
-        <v>29.19</v>
-      </c>
-      <c r="R86" s="3">
-        <v>25.4</v>
-      </c>
-      <c r="S86" s="3">
-        <v>27.52</v>
-      </c>
-      <c r="T86" s="3">
-        <v>25.4</v>
-      </c>
-      <c r="U86" s="3">
-        <v>27.36</v>
-      </c>
-    </row>
-    <row r="87" spans="1:65" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="2">
-        <v>43998.339227928242</v>
-      </c>
-      <c r="B87" s="3" t="s">
-        <v>296</v>
-      </c>
-      <c r="C87" s="3" t="s">
-        <v>254</v>
-      </c>
-      <c r="E87" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="F87" s="4" t="s">
         <v>297</v>
       </c>
-      <c r="G87" s="3" t="s">
+      <c r="V82" s="3" t="s">
         <v>298</v>
       </c>
-      <c r="BI87" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="BJ87" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="BK87" s="3" t="s">
+      <c r="W82" s="3" t="s">
         <v>299</v>
       </c>
-      <c r="BL87" s="3" t="s">
-        <v>299</v>
-      </c>
-      <c r="BM87" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="88" spans="1:65" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="2">
-        <v>43998.340830671295</v>
-      </c>
-      <c r="B88" s="3" t="s">
-        <v>296</v>
-      </c>
-      <c r="C88" s="3" t="s">
-        <v>254</v>
-      </c>
-      <c r="E88" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F88" s="4" t="s">
+      <c r="X82" s="3" t="s">
         <v>300</v>
       </c>
-      <c r="O88" s="3">
-        <v>51.54</v>
-      </c>
-      <c r="P88" s="3">
-        <v>35.299999999999997</v>
-      </c>
-      <c r="Q88" s="3">
-        <v>35.11</v>
-      </c>
-      <c r="R88" s="3">
-        <v>32.979999999999997</v>
-      </c>
-      <c r="S88" s="3">
-        <v>28.59</v>
-      </c>
-      <c r="T88" s="3">
-        <v>28.59</v>
-      </c>
-      <c r="U88" s="3">
-        <v>34.46</v>
-      </c>
-    </row>
-    <row r="89" spans="1:65" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="2">
-        <v>43998.341803854171</v>
-      </c>
-      <c r="B89" s="3" t="s">
-        <v>296</v>
-      </c>
-      <c r="C89" s="3" t="s">
-        <v>254</v>
-      </c>
-      <c r="E89" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F89" s="4" t="s">
+      <c r="Y82" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z82" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA82" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="AB82" s="5" t="s">
         <v>301</v>
       </c>
-      <c r="V89" s="3" t="s">
-        <v>302</v>
-      </c>
-      <c r="W89" s="3" t="s">
-        <v>303</v>
-      </c>
-      <c r="X89" s="3" t="s">
-        <v>304</v>
-      </c>
-      <c r="Y89" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="Z89" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="AA89" s="3" t="s">
-        <v>304</v>
-      </c>
-      <c r="AB89" s="5" t="s">
-        <v>305</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:BW89" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="Alex Friedman"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:BW82" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="F3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
@@ -4864,50 +4568,48 @@
     <hyperlink ref="F38" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
     <hyperlink ref="F39" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
     <hyperlink ref="F40" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
-    <hyperlink ref="F41" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink ref="F42" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
-    <hyperlink ref="F43" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
-    <hyperlink ref="F44" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
-    <hyperlink ref="F45" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
-    <hyperlink ref="F46" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
-    <hyperlink ref="F47" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
-    <hyperlink ref="F48" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
-    <hyperlink ref="F49" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
-    <hyperlink ref="F50" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
-    <hyperlink ref="F51" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
-    <hyperlink ref="F52" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
-    <hyperlink ref="F53" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
-    <hyperlink ref="F54" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
-    <hyperlink ref="F60" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
-    <hyperlink ref="F61" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
-    <hyperlink ref="F62" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
-    <hyperlink ref="F63" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
-    <hyperlink ref="F64" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
-    <hyperlink ref="F65" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
-    <hyperlink ref="F66" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
-    <hyperlink ref="F67" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
-    <hyperlink ref="F68" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
-    <hyperlink ref="F69" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
-    <hyperlink ref="F70" r:id="rId64" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
-    <hyperlink ref="F71" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
-    <hyperlink ref="F72" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
-    <hyperlink ref="F73" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
-    <hyperlink ref="F74" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
-    <hyperlink ref="F75" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
-    <hyperlink ref="F76" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
-    <hyperlink ref="F77" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
-    <hyperlink ref="F78" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
-    <hyperlink ref="F79" r:id="rId73" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
-    <hyperlink ref="F80" r:id="rId74" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
-    <hyperlink ref="F81" r:id="rId75" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
-    <hyperlink ref="F82" r:id="rId76" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
-    <hyperlink ref="F83" r:id="rId77" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
-    <hyperlink ref="F84" r:id="rId78" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
-    <hyperlink ref="F85" r:id="rId79" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
-    <hyperlink ref="F86" r:id="rId80" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
-    <hyperlink ref="F87" r:id="rId81" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
-    <hyperlink ref="F88" r:id="rId82" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
-    <hyperlink ref="F89" r:id="rId83" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
+    <hyperlink ref="F41" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="F42" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="F43" r:id="rId42" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="F44" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="F45" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="F46" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="F47" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="F48" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="F49" r:id="rId48" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="F50" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="F51" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="F52" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="F53" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="F54" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="F55" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="F56" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="F57" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="F58" r:id="rId57" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="F59" r:id="rId58" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="F60" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="F61" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="F62" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink ref="F63" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink ref="F64" r:id="rId63" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="F65" r:id="rId64" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="F66" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
+    <hyperlink ref="F67" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
+    <hyperlink ref="F68" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
+    <hyperlink ref="F69" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
+    <hyperlink ref="F70" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
+    <hyperlink ref="F71" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
+    <hyperlink ref="F72" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
+    <hyperlink ref="F73" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
+    <hyperlink ref="F74" r:id="rId73" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
+    <hyperlink ref="F75" r:id="rId74" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
+    <hyperlink ref="F76" r:id="rId75" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
+    <hyperlink ref="F77" r:id="rId76" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
+    <hyperlink ref="F78" r:id="rId77" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
+    <hyperlink ref="F79" r:id="rId78" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
+    <hyperlink ref="F80" r:id="rId79" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
+    <hyperlink ref="F81" r:id="rId80" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
+    <hyperlink ref="F82" r:id="rId81" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>